<commit_message>
feat: Update mentors details in automation.py script
Update samples yml and xlsx files
</commit_message>
<xml_diff>
--- a/tools/samples/mentors.xlsx
+++ b/tools/samples/mentors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>Timestamp</t>
   </si>
@@ -150,13 +150,16 @@
     <t>Are you happy for us to highlight/promote you as our mentor on our social media?</t>
   </si>
   <si>
-    <t>Arzu Caner</t>
+    <t>Mentor2 Name</t>
   </si>
   <si>
     <t>anyemail2@mail.com</t>
   </si>
   <si>
     <t>Ad-Hoc Format</t>
+  </si>
+  <si>
+    <t>Mentor2</t>
   </si>
   <si>
     <t>United Kingdom/London</t>
@@ -194,7 +197,7 @@
     <t>Those who are changing their careers, interested in app development.</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/arzucaner/</t>
+    <t>https://www.linkedin.com/in/mentor2/</t>
   </si>
   <si>
     <t>https://x.com/arz_ugny, https://arzugny.medium.com/, https://github.com/arzucaner, https://www.youtube.com/channel/UCsK0v6RouRYb5I1Ny8flrOg</t>
@@ -218,7 +221,7 @@
     <t>September, October, November</t>
   </si>
   <si>
-    <t xml:space="preserve">Marie Coquille </t>
+    <t>Mentor3 Name</t>
   </si>
   <si>
     <t>anyemail1@mail.com</t>
@@ -227,7 +230,7 @@
     <t>Both</t>
   </si>
   <si>
-    <t>marie</t>
+    <t>Mentor3</t>
   </si>
   <si>
     <t>London, UK</t>
@@ -263,7 +266,7 @@
     <t>Juniors.</t>
   </si>
   <si>
-    <t>https://uk.linkedin.com/in/marie-coquille-b0b733100</t>
+    <t>https://uk.linkedin.com/in/mentor3</t>
   </si>
   <si>
     <t>I'd rather do all of that once we know if I'm joining as a mentor?</t>
@@ -305,7 +308,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -396,7 +399,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,86 +958,86 @@
         <v>46</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AE2" s="7">
         <v>2</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AK2" s="6"/>
       <c r="AL2" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AM2" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AP2" s="6"/>
       <c r="AQ2" s="6"/>
@@ -1072,49 +1075,49 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1126,48 +1129,48 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE3" s="7">
         <v>4</v>
       </c>
       <c r="AF3" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AK3" s="6"/>
       <c r="AL3" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO3" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AP3" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AQ3" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AR3" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AS3" s="6"/>
       <c r="AT3" s="6"/>
@@ -1196,7 +1199,7 @@
       <c r="BQ3" s="6"/>
       <c r="BR3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1268,7 +1271,7 @@
       <c r="BQ4" s="9"/>
       <c r="BR4" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>

</xml_diff>

<commit_message>
update mentor_addition automation tool for use during long-term reg. versus default (ad-hoc) periods
</commit_message>
<xml_diff>
--- a/tools/samples/mentors.xlsx
+++ b/tools/samples/mentors.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airah/Desktop/WCC/wcc/tools/samples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C625DE-7BFD-E446-ACB9-0FAB18FAEE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="24600" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="WCC All Approved Mentors"/>
+    <sheet name="WCC All Approved Mentors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Timestamp</t>
   </si>
@@ -281,16 +287,19 @@
   </si>
   <si>
     <t>She / her</t>
+  </si>
+  <si>
+    <t>How many mentees would you be able to mentor? (Long-term only)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,7 +316,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000ff"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -315,6 +324,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -327,7 +342,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -348,16 +363,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -365,56 +380,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -425,10 +438,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -466,71 +479,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -558,7 +571,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -581,11 +594,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -594,13 +607,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -610,7 +623,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -619,7 +632,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -628,7 +641,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -636,10 +649,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -704,91 +717,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="11" width="29.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="50.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="12" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="12" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="13" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="12" width="99.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="12" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="12" width="57.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="12" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="12" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="12" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="12" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="12" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="12" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="12" width="34.005" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="64" max="64" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="65" max="65" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="66" max="66" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="67" max="67" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="68" max="68" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="69" max="69" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="70" max="70" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="99.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="31" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="34" bestFit="1" customWidth="1"/>
+    <col min="45" max="70" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="126.75">
+    <row r="1" spans="1:70" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +897,9 @@
       <c r="AR1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2"/>
+      <c r="AS1" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
       <c r="AV1" s="2"/>
@@ -948,7 +926,7 @@
       <c r="BQ1" s="2"/>
       <c r="BR1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="69.75">
+    <row r="2" spans="1:70" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>45537.933969907404</v>
       </c>
@@ -1047,34 +1025,15 @@
       <c r="AP2" s="6"/>
       <c r="AQ2" s="6"/>
       <c r="AR2" s="6"/>
-      <c r="AS2" s="6"/>
+      <c r="AS2" s="6">
+        <v>1</v>
+      </c>
       <c r="AT2" s="6"/>
       <c r="AU2" s="6"/>
       <c r="AV2" s="6"/>
       <c r="AW2" s="6"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9"/>
-      <c r="BN2" s="9"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="9"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25">
+    <row r="3" spans="1:70" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>45668.018483796295</v>
       </c>
@@ -1179,7 +1138,9 @@
       <c r="AR3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AS3" s="6"/>
+      <c r="AS3" s="6">
+        <v>2</v>
+      </c>
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
@@ -1206,151 +1167,16 @@
       <c r="BQ3" s="6"/>
       <c r="BR3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9"/>
-      <c r="AT4" s="9"/>
-      <c r="AU4" s="9"/>
-      <c r="AV4" s="9"/>
-      <c r="AW4" s="9"/>
-      <c r="AX4" s="9"/>
-      <c r="AY4" s="9"/>
-      <c r="AZ4" s="9"/>
-      <c r="BA4" s="9"/>
-      <c r="BB4" s="9"/>
-      <c r="BC4" s="9"/>
-      <c r="BD4" s="9"/>
-      <c r="BE4" s="9"/>
-      <c r="BF4" s="9"/>
-      <c r="BG4" s="9"/>
-      <c r="BH4" s="9"/>
-      <c r="BI4" s="9"/>
-      <c r="BJ4" s="9"/>
-      <c r="BK4" s="9"/>
-      <c r="BL4" s="9"/>
-      <c r="BM4" s="9"/>
-      <c r="BN4" s="9"/>
-      <c r="BO4" s="9"/>
-      <c r="BP4" s="9"/>
-      <c r="BQ4" s="9"/>
-      <c r="BR4" s="9"/>
+      <c r="AE4" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="9"/>
-      <c r="AU5" s="9"/>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9"/>
-      <c r="AX5" s="9"/>
-      <c r="AY5" s="9"/>
-      <c r="AZ5" s="9"/>
-      <c r="BA5" s="9"/>
-      <c r="BB5" s="9"/>
-      <c r="BC5" s="9"/>
-      <c r="BD5" s="9"/>
-      <c r="BE5" s="9"/>
-      <c r="BF5" s="9"/>
-      <c r="BG5" s="9"/>
-      <c r="BH5" s="9"/>
-      <c r="BI5" s="9"/>
-      <c r="BJ5" s="9"/>
-      <c r="BK5" s="9"/>
-      <c r="BL5" s="9"/>
-      <c r="BM5" s="9"/>
-      <c r="BN5" s="9"/>
-      <c r="BO5" s="9"/>
-      <c r="BP5" s="9"/>
-      <c r="BQ5" s="9"/>
-      <c r="BR5" s="9"/>
+      <c r="AE5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx file should include num_mentees column data
</commit_message>
<xml_diff>
--- a/tools/samples/mentors.xlsx
+++ b/tools/samples/mentors.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airah/Desktop/WCC/wcc/tools/samples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C625DE-7BFD-E446-ACB9-0FAB18FAEE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="24600" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="WCC All Approved Mentors"/>
+    <sheet name="WCC All Approved Mentors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Timestamp</t>
   </si>
@@ -281,16 +287,19 @@
   </si>
   <si>
     <t>She / her</t>
+  </si>
+  <si>
+    <t>How many mentees would you be able to mentor? (Long-term only)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,7 +316,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000ff"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -315,6 +324,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -327,7 +342,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -348,16 +363,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -365,56 +380,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -425,10 +438,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -466,71 +479,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -558,7 +571,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -581,11 +594,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -594,13 +607,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -610,7 +623,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -619,7 +632,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -628,7 +641,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -636,10 +649,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -704,91 +717,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="11" width="29.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="50.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="12" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="12" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="13" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="12" width="99.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="12" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="12" width="57.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="12" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="12" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="12" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="12" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="12" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="12" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="12" width="34.005" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="64" max="64" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="65" max="65" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="66" max="66" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="67" max="67" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="68" max="68" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="69" max="69" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="70" max="70" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="99.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="31" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="34" bestFit="1" customWidth="1"/>
+    <col min="45" max="70" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="126.75">
+    <row r="1" spans="1:70" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +897,9 @@
       <c r="AR1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2"/>
+      <c r="AS1" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
       <c r="AV1" s="2"/>
@@ -948,7 +926,7 @@
       <c r="BQ1" s="2"/>
       <c r="BR1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="69.75">
+    <row r="2" spans="1:70" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>45537.933969907404</v>
       </c>
@@ -1047,34 +1025,15 @@
       <c r="AP2" s="6"/>
       <c r="AQ2" s="6"/>
       <c r="AR2" s="6"/>
-      <c r="AS2" s="6"/>
+      <c r="AS2" s="6">
+        <v>1</v>
+      </c>
       <c r="AT2" s="6"/>
       <c r="AU2" s="6"/>
       <c r="AV2" s="6"/>
       <c r="AW2" s="6"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9"/>
-      <c r="BN2" s="9"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="9"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25">
+    <row r="3" spans="1:70" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>45668.018483796295</v>
       </c>
@@ -1179,7 +1138,9 @@
       <c r="AR3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AS3" s="6"/>
+      <c r="AS3" s="6">
+        <v>2</v>
+      </c>
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
@@ -1206,151 +1167,16 @@
       <c r="BQ3" s="6"/>
       <c r="BR3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9"/>
-      <c r="AT4" s="9"/>
-      <c r="AU4" s="9"/>
-      <c r="AV4" s="9"/>
-      <c r="AW4" s="9"/>
-      <c r="AX4" s="9"/>
-      <c r="AY4" s="9"/>
-      <c r="AZ4" s="9"/>
-      <c r="BA4" s="9"/>
-      <c r="BB4" s="9"/>
-      <c r="BC4" s="9"/>
-      <c r="BD4" s="9"/>
-      <c r="BE4" s="9"/>
-      <c r="BF4" s="9"/>
-      <c r="BG4" s="9"/>
-      <c r="BH4" s="9"/>
-      <c r="BI4" s="9"/>
-      <c r="BJ4" s="9"/>
-      <c r="BK4" s="9"/>
-      <c r="BL4" s="9"/>
-      <c r="BM4" s="9"/>
-      <c r="BN4" s="9"/>
-      <c r="BO4" s="9"/>
-      <c r="BP4" s="9"/>
-      <c r="BQ4" s="9"/>
-      <c r="BR4" s="9"/>
+      <c r="AE4" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="9"/>
-      <c r="AU5" s="9"/>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9"/>
-      <c r="AX5" s="9"/>
-      <c r="AY5" s="9"/>
-      <c r="AZ5" s="9"/>
-      <c r="BA5" s="9"/>
-      <c r="BB5" s="9"/>
-      <c r="BC5" s="9"/>
-      <c r="BD5" s="9"/>
-      <c r="BE5" s="9"/>
-      <c r="BF5" s="9"/>
-      <c r="BG5" s="9"/>
-      <c r="BH5" s="9"/>
-      <c r="BI5" s="9"/>
-      <c r="BJ5" s="9"/>
-      <c r="BK5" s="9"/>
-      <c r="BL5" s="9"/>
-      <c r="BM5" s="9"/>
-      <c r="BN5" s="9"/>
-      <c r="BO5" s="9"/>
-      <c r="BP5" s="9"/>
-      <c r="BQ5" s="9"/>
-      <c r="BR5" s="9"/>
+      <c r="AE5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update download_image script to use excel file and download images for all rows + readme update
</commit_message>
<xml_diff>
--- a/tools/samples/mentors.xlsx
+++ b/tools/samples/mentors.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airah/Desktop/WCC/wcc/tools/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C625DE-7BFD-E446-ACB9-0FAB18FAEE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C820DFB5-DBA2-5448-BC39-A4ADA424FD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="24600" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="24600" windowHeight="13300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WCC All Approved Mentors" sheetId="1" r:id="rId1"/>
+    <sheet name="WCC Approved Mentors" sheetId="1" r:id="rId1"/>
+    <sheet name="Mentors Images" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>Timestamp</t>
   </si>
@@ -156,9 +157,6 @@
     <t>Are you happy for us to highlight/promote you as our mentor on our social media?</t>
   </si>
   <si>
-    <t xml:space="preserve">   Mentor2 Name   </t>
-  </si>
-  <si>
     <t>anyemail2@mail.com</t>
   </si>
   <si>
@@ -290,6 +288,21 @@
   </si>
   <si>
     <t>How many mentees would you be able to mentor? (Long-term only)</t>
+  </si>
+  <si>
+    <t>Mentor Name</t>
+  </si>
+  <si>
+    <t>Image Download URL</t>
+  </si>
+  <si>
+    <t>https://media.licdn.com/media/AAYQBAT4AAgAAQAAAAAAAEGGOGBx-2JrSbmYjhlTsMoxwg.png</t>
+  </si>
+  <si>
+    <t>https://ca.slack-edge.com/T070P4KN0P2-U09GHR2AWNB-2758bb05eaba-512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mentor2 Name   </t>
   </si>
 </sst>
 </file>
@@ -723,9 +736,9 @@
   </sheetPr>
   <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR7" sqref="AR7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -761,7 +774,8 @@
     <col min="42" max="42" width="34.83203125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="31" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="34" bestFit="1" customWidth="1"/>
-    <col min="45" max="70" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="13.5" customWidth="1"/>
+    <col min="47" max="70" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,7 +912,7 @@
         <v>43</v>
       </c>
       <c r="AS1" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
@@ -932,95 +946,95 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE2" s="7">
         <v>2</v>
       </c>
       <c r="AF2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AI2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="AK2" s="6"/>
       <c r="AL2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AM2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="AO2" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="AP2" s="6"/>
       <c r="AQ2" s="6"/>
@@ -1039,49 +1053,49 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1093,50 +1107,50 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AE3" s="7">
         <v>4</v>
       </c>
       <c r="AF3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AH3" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="AI3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK3" s="6"/>
       <c r="AL3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AO3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AP3" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="AQ3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AR3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AS3" s="6">
         <v>2</v>
@@ -1179,4 +1193,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4025B5B2-1104-AA4C-A926-33B7646E044E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: sheet names should match usage in script
</commit_message>
<xml_diff>
--- a/tools/samples/mentors.xlsx
+++ b/tools/samples/mentors.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airah/Desktop/WCC/wcc/tools/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C820DFB5-DBA2-5448-BC39-A4ADA424FD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7050DF-CE94-CD40-B123-762BEB342998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="24600" windowHeight="13300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="24600" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WCC Approved Mentors" sheetId="1" r:id="rId1"/>
+    <sheet name="WCC All Approved Mentors" sheetId="1" r:id="rId1"/>
     <sheet name="Mentors Images" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -736,7 +736,7 @@
   </sheetPr>
   <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
     </sheetView>
@@ -1199,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4025B5B2-1104-AA4C-A926-33B7646E044E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>